<commit_message>
Change some view's layout
</commit_message>
<xml_diff>
--- a/Standard/Training/Training Arrangement.xlsx
+++ b/Standard/Training/Training Arrangement.xlsx
@@ -137,57 +137,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2017.7.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017.7.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017.7.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017.7.4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Teaching
 &amp;
 Show-how</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017.7.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017.7.6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017.7.7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017.7.8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017.7.9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017.7.10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017.7.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017.7.12</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -216,12 +168,60 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>2017.7.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.7.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.7.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.7.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.7.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.7.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.7.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.7.9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.7.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.7.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.7.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.7.13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +308,13 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1235,15 +1242,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1314,6 +1312,54 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="10" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1331,36 +1377,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1436,97 +1455,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1538,31 +1482,94 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1965,83 +1972,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="75"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="76"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="69"/>
+      <c r="Y1" s="70"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4">
         <v>42891</v>
       </c>
-      <c r="C2" s="77">
+      <c r="C2" s="75">
         <v>42892</v>
       </c>
-      <c r="D2" s="78"/>
-      <c r="E2" s="77">
+      <c r="D2" s="76"/>
+      <c r="E2" s="75">
         <v>42893</v>
       </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="65">
+      <c r="F2" s="76"/>
+      <c r="G2" s="78">
         <v>42894</v>
       </c>
-      <c r="H2" s="65"/>
-      <c r="I2" s="69">
+      <c r="H2" s="78"/>
+      <c r="I2" s="73">
         <v>42895</v>
       </c>
-      <c r="J2" s="70"/>
+      <c r="J2" s="82"/>
       <c r="K2" s="71">
         <v>42896</v>
       </c>
       <c r="L2" s="72"/>
-      <c r="M2" s="69">
+      <c r="M2" s="73">
         <v>42897</v>
       </c>
-      <c r="N2" s="73"/>
+      <c r="N2" s="74"/>
       <c r="O2" s="71">
         <v>42898</v>
       </c>
       <c r="P2" s="72"/>
-      <c r="Q2" s="69">
+      <c r="Q2" s="73">
         <v>42899</v>
       </c>
-      <c r="R2" s="73"/>
+      <c r="R2" s="74"/>
       <c r="S2" s="71">
         <v>42900</v>
       </c>
       <c r="T2" s="72"/>
-      <c r="U2" s="69">
+      <c r="U2" s="73">
         <v>42901</v>
       </c>
-      <c r="V2" s="73"/>
+      <c r="V2" s="74"/>
       <c r="W2" s="71">
         <v>42902</v>
       </c>
-      <c r="X2" s="73"/>
+      <c r="X2" s="74"/>
       <c r="Y2" s="5">
         <v>42903</v>
       </c>
@@ -2053,14 +2060,14 @@
       <c r="B3" s="14">
         <v>2000</v>
       </c>
-      <c r="C3" s="106">
+      <c r="C3" s="63">
         <v>3000</v>
       </c>
-      <c r="D3" s="107"/>
-      <c r="E3" s="106">
+      <c r="D3" s="64"/>
+      <c r="E3" s="63">
         <v>4000</v>
       </c>
-      <c r="F3" s="107"/>
+      <c r="F3" s="64"/>
       <c r="G3" s="16">
         <v>3000</v>
       </c>
@@ -2073,12 +2080,12 @@
       <c r="J3" s="24">
         <v>2000</v>
       </c>
-      <c r="K3" s="99" t="s">
+      <c r="K3" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="103"/>
       <c r="O3" s="10">
         <v>1000</v>
       </c>
@@ -2091,21 +2098,21 @@
       <c r="R3" s="11">
         <v>4000</v>
       </c>
-      <c r="S3" s="64">
+      <c r="S3" s="77">
         <v>6000</v>
       </c>
-      <c r="T3" s="64"/>
+      <c r="T3" s="77"/>
       <c r="U3" s="13">
         <v>2000</v>
       </c>
       <c r="V3" s="11">
         <v>3000</v>
       </c>
-      <c r="W3" s="109">
+      <c r="W3" s="66">
         <v>4000</v>
       </c>
-      <c r="X3" s="110"/>
-      <c r="Y3" s="66" t="s">
+      <c r="X3" s="67"/>
+      <c r="Y3" s="79" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2140,10 +2147,10 @@
       <c r="J4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="100"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="100"/>
+      <c r="K4" s="104"/>
+      <c r="L4" s="104"/>
+      <c r="M4" s="104"/>
+      <c r="N4" s="104"/>
       <c r="O4" s="14" t="s">
         <v>7</v>
       </c>
@@ -2156,10 +2163,10 @@
       <c r="R4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="108" t="s">
+      <c r="S4" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="108"/>
+      <c r="T4" s="65"/>
       <c r="U4" s="17" t="s">
         <v>10</v>
       </c>
@@ -2172,7 +2179,7 @@
       <c r="X4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="Y4" s="67"/>
+      <c r="Y4" s="80"/>
     </row>
     <row r="5" spans="1:25" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
@@ -2205,10 +2212,10 @@
       <c r="J5" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="100"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="104"/>
+      <c r="N5" s="104"/>
       <c r="O5" s="19" t="s">
         <v>18</v>
       </c>
@@ -2221,10 +2228,10 @@
       <c r="R5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="S5" s="105" t="s">
+      <c r="S5" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="T5" s="105"/>
+      <c r="T5" s="62"/>
       <c r="U5" s="21" t="s">
         <v>16</v>
       </c>
@@ -2237,169 +2244,153 @@
       <c r="X5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="67"/>
+      <c r="Y5" s="80"/>
     </row>
     <row r="6" spans="1:25" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="102"/>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="100"/>
-      <c r="O6" s="104"/>
-      <c r="P6" s="104"/>
-      <c r="Q6" s="104"/>
-      <c r="R6" s="104"/>
-      <c r="S6" s="104"/>
-      <c r="T6" s="104"/>
-      <c r="U6" s="104"/>
-      <c r="V6" s="104"/>
-      <c r="W6" s="104"/>
-      <c r="X6" s="104"/>
-      <c r="Y6" s="67"/>
+      <c r="A6" s="106"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="104"/>
+      <c r="L6" s="104"/>
+      <c r="M6" s="104"/>
+      <c r="N6" s="104"/>
+      <c r="O6" s="61"/>
+      <c r="P6" s="61"/>
+      <c r="Q6" s="61"/>
+      <c r="R6" s="61"/>
+      <c r="S6" s="61"/>
+      <c r="T6" s="61"/>
+      <c r="U6" s="61"/>
+      <c r="V6" s="61"/>
+      <c r="W6" s="61"/>
+      <c r="X6" s="61"/>
+      <c r="Y6" s="80"/>
     </row>
     <row r="7" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="100"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="100"/>
-      <c r="N7" s="100"/>
-      <c r="O7" s="91"/>
-      <c r="P7" s="86"/>
-      <c r="Q7" s="86"/>
-      <c r="R7" s="86"/>
-      <c r="S7" s="86"/>
-      <c r="T7" s="86"/>
-      <c r="U7" s="86"/>
-      <c r="V7" s="86"/>
-      <c r="W7" s="86"/>
-      <c r="X7" s="87"/>
-      <c r="Y7" s="67"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="104"/>
+      <c r="L7" s="104"/>
+      <c r="M7" s="104"/>
+      <c r="N7" s="104"/>
+      <c r="O7" s="95"/>
+      <c r="P7" s="90"/>
+      <c r="Q7" s="90"/>
+      <c r="R7" s="90"/>
+      <c r="S7" s="90"/>
+      <c r="T7" s="90"/>
+      <c r="U7" s="90"/>
+      <c r="V7" s="90"/>
+      <c r="W7" s="90"/>
+      <c r="X7" s="91"/>
+      <c r="Y7" s="80"/>
     </row>
     <row r="8" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="88"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="89"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="100"/>
-      <c r="L8" s="100"/>
-      <c r="M8" s="100"/>
-      <c r="N8" s="100"/>
-      <c r="O8" s="92"/>
-      <c r="P8" s="89"/>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="89"/>
-      <c r="S8" s="89"/>
-      <c r="T8" s="89"/>
-      <c r="U8" s="89"/>
-      <c r="V8" s="89"/>
-      <c r="W8" s="89"/>
-      <c r="X8" s="90"/>
-      <c r="Y8" s="67"/>
+      <c r="B8" s="92"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="93"/>
+      <c r="H8" s="93"/>
+      <c r="I8" s="93"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="104"/>
+      <c r="O8" s="96"/>
+      <c r="P8" s="93"/>
+      <c r="Q8" s="93"/>
+      <c r="R8" s="93"/>
+      <c r="S8" s="93"/>
+      <c r="T8" s="93"/>
+      <c r="U8" s="93"/>
+      <c r="V8" s="93"/>
+      <c r="W8" s="93"/>
+      <c r="X8" s="94"/>
+      <c r="Y8" s="80"/>
     </row>
     <row r="9" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="82"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="100"/>
-      <c r="L9" s="100"/>
-      <c r="M9" s="100"/>
-      <c r="N9" s="100"/>
-      <c r="O9" s="93"/>
-      <c r="P9" s="94"/>
-      <c r="Q9" s="94"/>
-      <c r="R9" s="94"/>
-      <c r="S9" s="94"/>
-      <c r="T9" s="94"/>
-      <c r="U9" s="94"/>
-      <c r="V9" s="94"/>
-      <c r="W9" s="94"/>
-      <c r="X9" s="95"/>
-      <c r="Y9" s="67"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="88"/>
+      <c r="K9" s="104"/>
+      <c r="L9" s="104"/>
+      <c r="M9" s="104"/>
+      <c r="N9" s="104"/>
+      <c r="O9" s="97"/>
+      <c r="P9" s="98"/>
+      <c r="Q9" s="98"/>
+      <c r="R9" s="98"/>
+      <c r="S9" s="98"/>
+      <c r="T9" s="98"/>
+      <c r="U9" s="98"/>
+      <c r="V9" s="98"/>
+      <c r="W9" s="98"/>
+      <c r="X9" s="99"/>
+      <c r="Y9" s="80"/>
     </row>
     <row r="10" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="101"/>
-      <c r="M10" s="101"/>
-      <c r="N10" s="101"/>
-      <c r="O10" s="96"/>
-      <c r="P10" s="97"/>
-      <c r="Q10" s="97"/>
-      <c r="R10" s="97"/>
-      <c r="S10" s="97"/>
-      <c r="T10" s="97"/>
-      <c r="U10" s="97"/>
-      <c r="V10" s="97"/>
-      <c r="W10" s="97"/>
-      <c r="X10" s="98"/>
-      <c r="Y10" s="68"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="84"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="105"/>
+      <c r="M10" s="105"/>
+      <c r="N10" s="105"/>
+      <c r="O10" s="100"/>
+      <c r="P10" s="101"/>
+      <c r="Q10" s="101"/>
+      <c r="R10" s="101"/>
+      <c r="S10" s="101"/>
+      <c r="T10" s="101"/>
+      <c r="U10" s="101"/>
+      <c r="V10" s="101"/>
+      <c r="W10" s="101"/>
+      <c r="X10" s="102"/>
+      <c r="Y10" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="O6:X6"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="G2:H2"/>
     <mergeCell ref="Y3:Y10"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
@@ -2414,6 +2405,22 @@
     <mergeCell ref="O10:X10"/>
     <mergeCell ref="K3:N10"/>
     <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="O6:X6"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="S3:T3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2426,7 +2433,7 @@
   <dimension ref="B1:X11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:X2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2441,7 +2448,7 @@
     <row r="1" spans="2:24" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:24" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B2" s="144" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C2" s="145"/>
       <c r="D2" s="145"/>
@@ -2469,374 +2476,390 @@
     <row r="3" spans="2:24" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="30"/>
       <c r="C3" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="140" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="141"/>
-      <c r="F3" s="142" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="143"/>
-      <c r="H3" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="141"/>
-      <c r="J3" s="140" t="s">
+      <c r="D3" s="108" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="109"/>
+      <c r="F3" s="110" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="141"/>
-      <c r="L3" s="142" t="s">
+      <c r="G3" s="111"/>
+      <c r="H3" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="143"/>
-      <c r="N3" s="140" t="s">
+      <c r="I3" s="109"/>
+      <c r="J3" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="141"/>
-      <c r="P3" s="142" t="s">
+      <c r="K3" s="109"/>
+      <c r="L3" s="110" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="143"/>
-      <c r="R3" s="140" t="s">
+      <c r="M3" s="111"/>
+      <c r="N3" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="141"/>
-      <c r="T3" s="140" t="s">
+      <c r="O3" s="109"/>
+      <c r="P3" s="110" t="s">
         <v>39</v>
       </c>
-      <c r="U3" s="141"/>
-      <c r="V3" s="142" t="s">
+      <c r="Q3" s="111"/>
+      <c r="R3" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="W3" s="143"/>
-      <c r="X3" s="63" t="s">
+      <c r="S3" s="109"/>
+      <c r="T3" s="108" t="s">
         <v>41</v>
+      </c>
+      <c r="U3" s="109"/>
+      <c r="V3" s="110" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="111"/>
+      <c r="X3" s="60" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:24" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="118" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="115">
+      <c r="C4" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="117">
         <v>2000</v>
       </c>
-      <c r="E4" s="116"/>
-      <c r="F4" s="136">
+      <c r="E4" s="118"/>
+      <c r="F4" s="115">
         <v>3000</v>
       </c>
-      <c r="G4" s="137"/>
-      <c r="H4" s="115">
+      <c r="G4" s="116"/>
+      <c r="H4" s="117">
         <v>4000</v>
       </c>
-      <c r="I4" s="116"/>
-      <c r="J4" s="50">
+      <c r="I4" s="118"/>
+      <c r="J4" s="47">
         <v>3000</v>
       </c>
-      <c r="K4" s="51">
+      <c r="K4" s="48">
         <v>1000</v>
       </c>
-      <c r="L4" s="44">
+      <c r="L4" s="41">
         <v>2000</v>
       </c>
-      <c r="M4" s="52">
+      <c r="M4" s="49">
         <v>2000</v>
       </c>
-      <c r="N4" s="56">
+      <c r="N4" s="53">
         <v>1000</v>
       </c>
-      <c r="O4" s="51">
+      <c r="O4" s="48">
         <v>3000</v>
       </c>
-      <c r="P4" s="54">
+      <c r="P4" s="51">
         <v>1000</v>
       </c>
-      <c r="Q4" s="52">
+      <c r="Q4" s="49">
         <v>4000</v>
       </c>
-      <c r="R4" s="115">
+      <c r="R4" s="117">
         <v>6000</v>
       </c>
-      <c r="S4" s="116"/>
-      <c r="T4" s="56">
+      <c r="S4" s="118"/>
+      <c r="T4" s="53">
         <v>2000</v>
       </c>
-      <c r="U4" s="51">
+      <c r="U4" s="48">
         <v>3000</v>
       </c>
-      <c r="V4" s="138">
+      <c r="V4" s="119">
         <v>4000</v>
       </c>
-      <c r="W4" s="139"/>
-      <c r="X4" s="118" t="s">
-        <v>42</v>
+      <c r="W4" s="120"/>
+      <c r="X4" s="112" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:24" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="119"/>
-      <c r="D5" s="113" t="s">
+      <c r="C5" s="126"/>
+      <c r="D5" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="F5" s="40" t="s">
+      <c r="E5" s="124"/>
+      <c r="F5" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="46" t="s">
+      <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="46" t="s">
+      <c r="K5" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="49" t="s">
+      <c r="L5" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="53" t="s">
+      <c r="M5" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="45" t="s">
+      <c r="N5" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="57" t="s">
+      <c r="O5" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="40" t="s">
+      <c r="P5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="53" t="s">
+      <c r="Q5" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="R5" s="130" t="s">
+      <c r="R5" s="137" t="s">
         <v>4</v>
       </c>
-      <c r="S5" s="131"/>
-      <c r="T5" s="61" t="s">
+      <c r="S5" s="138"/>
+      <c r="T5" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="U5" s="57" t="s">
+      <c r="U5" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="V5" s="49" t="s">
+      <c r="V5" s="46" t="s">
         <v>9</v>
       </c>
       <c r="W5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="X5" s="134"/>
+      <c r="X5" s="113"/>
     </row>
     <row r="6" spans="2:24" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="119"/>
-      <c r="D6" s="111" t="s">
+      <c r="C6" s="126"/>
+      <c r="D6" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="112"/>
-      <c r="F6" s="41" t="s">
+      <c r="E6" s="122"/>
+      <c r="F6" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="43" t="s">
+      <c r="G6" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="48" t="s">
+      <c r="I6" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="47" t="s">
+      <c r="J6" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="48" t="s">
+      <c r="K6" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="41" t="s">
+      <c r="L6" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="43" t="s">
+      <c r="M6" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="47" t="s">
+      <c r="N6" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="58" t="s">
+      <c r="O6" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="P6" s="55" t="s">
+      <c r="P6" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" s="59" t="s">
+      <c r="Q6" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="R6" s="132" t="s">
+      <c r="R6" s="139" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="133"/>
-      <c r="T6" s="62" t="s">
+      <c r="S6" s="140"/>
+      <c r="T6" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="U6" s="58" t="s">
+      <c r="U6" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="V6" s="60" t="s">
+      <c r="V6" s="57" t="s">
         <v>8</v>
       </c>
       <c r="W6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="X6" s="134"/>
+      <c r="X6" s="113"/>
     </row>
     <row r="7" spans="2:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B7" s="36"/>
-      <c r="C7" s="120"/>
-      <c r="D7" s="117"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="117"/>
-      <c r="H7" s="117"/>
-      <c r="I7" s="117"/>
-      <c r="J7" s="117"/>
-      <c r="K7" s="117"/>
-      <c r="L7" s="117"/>
-      <c r="M7" s="117"/>
-      <c r="N7" s="117"/>
-      <c r="O7" s="117"/>
-      <c r="P7" s="117"/>
-      <c r="Q7" s="117"/>
-      <c r="R7" s="117"/>
-      <c r="S7" s="117"/>
-      <c r="T7" s="117"/>
-      <c r="U7" s="117"/>
-      <c r="V7" s="117"/>
-      <c r="W7" s="117"/>
-      <c r="X7" s="134"/>
+      <c r="C7" s="127"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="125"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="125"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="125"/>
+      <c r="M7" s="125"/>
+      <c r="N7" s="125"/>
+      <c r="O7" s="125"/>
+      <c r="P7" s="125"/>
+      <c r="Q7" s="125"/>
+      <c r="R7" s="125"/>
+      <c r="S7" s="125"/>
+      <c r="T7" s="125"/>
+      <c r="U7" s="125"/>
+      <c r="V7" s="125"/>
+      <c r="W7" s="125"/>
+      <c r="X7" s="113"/>
     </row>
-    <row r="8" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="37" t="s">
+    <row r="8" spans="2:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="141" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="119"/>
-      <c r="D8" s="122"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="123"/>
-      <c r="G8" s="123"/>
-      <c r="H8" s="123"/>
-      <c r="I8" s="123"/>
-      <c r="J8" s="123"/>
-      <c r="K8" s="123"/>
-      <c r="L8" s="123"/>
-      <c r="M8" s="123"/>
-      <c r="N8" s="123"/>
-      <c r="O8" s="123"/>
-      <c r="P8" s="123"/>
-      <c r="Q8" s="123"/>
-      <c r="R8" s="123"/>
-      <c r="S8" s="123"/>
-      <c r="T8" s="123"/>
-      <c r="U8" s="123"/>
-      <c r="V8" s="123"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="134"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="130"/>
+      <c r="G8" s="130"/>
+      <c r="H8" s="130"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="130"/>
+      <c r="K8" s="130"/>
+      <c r="L8" s="130"/>
+      <c r="M8" s="130"/>
+      <c r="N8" s="130"/>
+      <c r="O8" s="130"/>
+      <c r="P8" s="130"/>
+      <c r="Q8" s="130"/>
+      <c r="R8" s="130"/>
+      <c r="S8" s="130"/>
+      <c r="T8" s="130"/>
+      <c r="U8" s="130"/>
+      <c r="V8" s="130"/>
+      <c r="W8" s="130"/>
+      <c r="X8" s="113"/>
     </row>
-    <row r="9" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="38" t="s">
+    <row r="9" spans="2:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="142" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="119"/>
-      <c r="D9" s="124"/>
-      <c r="E9" s="125"/>
-      <c r="F9" s="125"/>
-      <c r="G9" s="125"/>
-      <c r="H9" s="125"/>
-      <c r="I9" s="125"/>
-      <c r="J9" s="125"/>
-      <c r="K9" s="125"/>
-      <c r="L9" s="125"/>
-      <c r="M9" s="125"/>
-      <c r="N9" s="125"/>
-      <c r="O9" s="125"/>
-      <c r="P9" s="125"/>
-      <c r="Q9" s="125"/>
-      <c r="R9" s="125"/>
-      <c r="S9" s="125"/>
-      <c r="T9" s="125"/>
-      <c r="U9" s="125"/>
-      <c r="V9" s="125"/>
-      <c r="W9" s="125"/>
-      <c r="X9" s="134"/>
+      <c r="C9" s="126"/>
+      <c r="D9" s="131"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="132"/>
+      <c r="H9" s="132"/>
+      <c r="I9" s="132"/>
+      <c r="J9" s="132"/>
+      <c r="K9" s="132"/>
+      <c r="L9" s="132"/>
+      <c r="M9" s="132"/>
+      <c r="N9" s="132"/>
+      <c r="O9" s="132"/>
+      <c r="P9" s="132"/>
+      <c r="Q9" s="132"/>
+      <c r="R9" s="132"/>
+      <c r="S9" s="132"/>
+      <c r="T9" s="132"/>
+      <c r="U9" s="132"/>
+      <c r="V9" s="132"/>
+      <c r="W9" s="132"/>
+      <c r="X9" s="113"/>
     </row>
-    <row r="10" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="38" t="s">
+    <row r="10" spans="2:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="142" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="119"/>
-      <c r="D10" s="126"/>
-      <c r="E10" s="127"/>
-      <c r="F10" s="127"/>
-      <c r="G10" s="127"/>
-      <c r="H10" s="127"/>
-      <c r="I10" s="127"/>
-      <c r="J10" s="127"/>
-      <c r="K10" s="127"/>
-      <c r="L10" s="127"/>
-      <c r="M10" s="127"/>
-      <c r="N10" s="127"/>
-      <c r="O10" s="127"/>
-      <c r="P10" s="127"/>
-      <c r="Q10" s="127"/>
-      <c r="R10" s="127"/>
-      <c r="S10" s="127"/>
-      <c r="T10" s="127"/>
-      <c r="U10" s="127"/>
-      <c r="V10" s="127"/>
-      <c r="W10" s="127"/>
-      <c r="X10" s="134"/>
+      <c r="C10" s="126"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="134"/>
+      <c r="F10" s="134"/>
+      <c r="G10" s="134"/>
+      <c r="H10" s="134"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
+      <c r="K10" s="134"/>
+      <c r="L10" s="134"/>
+      <c r="M10" s="134"/>
+      <c r="N10" s="134"/>
+      <c r="O10" s="134"/>
+      <c r="P10" s="134"/>
+      <c r="Q10" s="134"/>
+      <c r="R10" s="134"/>
+      <c r="S10" s="134"/>
+      <c r="T10" s="134"/>
+      <c r="U10" s="134"/>
+      <c r="V10" s="134"/>
+      <c r="W10" s="134"/>
+      <c r="X10" s="113"/>
     </row>
-    <row r="11" spans="2:24" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="39" t="s">
+    <row r="11" spans="2:24" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="143" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="121"/>
-      <c r="D11" s="128"/>
-      <c r="E11" s="129"/>
-      <c r="F11" s="129"/>
-      <c r="G11" s="129"/>
-      <c r="H11" s="129"/>
-      <c r="I11" s="129"/>
-      <c r="J11" s="129"/>
-      <c r="K11" s="129"/>
-      <c r="L11" s="129"/>
-      <c r="M11" s="129"/>
-      <c r="N11" s="129"/>
-      <c r="O11" s="129"/>
-      <c r="P11" s="129"/>
-      <c r="Q11" s="129"/>
-      <c r="R11" s="129"/>
-      <c r="S11" s="129"/>
-      <c r="T11" s="129"/>
-      <c r="U11" s="129"/>
-      <c r="V11" s="129"/>
-      <c r="W11" s="129"/>
-      <c r="X11" s="135"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="135"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="136"/>
+      <c r="H11" s="136"/>
+      <c r="I11" s="136"/>
+      <c r="J11" s="136"/>
+      <c r="K11" s="136"/>
+      <c r="L11" s="136"/>
+      <c r="M11" s="136"/>
+      <c r="N11" s="136"/>
+      <c r="O11" s="136"/>
+      <c r="P11" s="136"/>
+      <c r="Q11" s="136"/>
+      <c r="R11" s="136"/>
+      <c r="S11" s="136"/>
+      <c r="T11" s="136"/>
+      <c r="U11" s="136"/>
+      <c r="V11" s="136"/>
+      <c r="W11" s="136"/>
+      <c r="X11" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D7:W7"/>
+    <mergeCell ref="C4:C11"/>
+    <mergeCell ref="D8:W8"/>
+    <mergeCell ref="D9:W9"/>
+    <mergeCell ref="D10:W10"/>
+    <mergeCell ref="D11:W11"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="V4:W4"/>
     <mergeCell ref="B2:X2"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
@@ -2848,22 +2871,6 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D7:W7"/>
-    <mergeCell ref="C4:C11"/>
-    <mergeCell ref="D8:W8"/>
-    <mergeCell ref="D9:W9"/>
-    <mergeCell ref="D10:W10"/>
-    <mergeCell ref="D11:W11"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="R6:S6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>